<commit_message>
Changing the marks name
</commit_message>
<xml_diff>
--- a/Marks.xlsx
+++ b/Marks.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspaces\Github\algorithmicsGarciaDiazVicenteUO42478\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UO293175\git\algorithmicsYildirimKutayUO293175\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CE8C83-ADD9-435A-848F-C323013A518B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="38625" windowHeight="21225"/>
   </bookViews>
   <sheets>
     <sheet name="Marks" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,21 +29,27 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={546631AC-B603-4F16-94FA-E61B5900ACC3}</author>
     <author>Vicente García Díaz</author>
   </authors>
   <commentList>
-    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{546631AC-B603-4F16-94FA-E61B5900ACC3}">
+    <comment ref="I5" authorId="0" shapeId="0">
       <text>
-        <t>[Comentario encadenado]
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     last day of labs</t>
+        </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="1" shapeId="0" xr:uid="{D2FE9B25-C79E-4D70-AA94-F447E6592842}">
+    <comment ref="J5" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -220,9 +225,6 @@
     </r>
   </si>
   <si>
-    <t>García Díaz, Vicente</t>
-  </si>
-  <si>
     <t>Maximum possible grade in labs = 7</t>
   </si>
   <si>
@@ -230,12 +232,15 @@
   </si>
   <si>
     <t>Weights</t>
+  </si>
+  <si>
+    <t>Kutay Yildirim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -412,7 +417,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -424,6 +428,14 @@
     <xf numFmtId="9" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -433,14 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,127 +453,10 @@
   <dxfs count="12">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="8"/>
-        </left>
-        <right style="thin">
-          <color indexed="8"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="8"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="8"/>
-        </left>
-        <right style="thin">
-          <color indexed="8"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="8"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="8"/>
-        </left>
-        <right style="thin">
-          <color indexed="8"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="8"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="8"/>
-        </left>
-        <right style="thin">
-          <color indexed="8"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="8"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="8"/>
-        </left>
-        <right style="thin">
-          <color indexed="8"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="8"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="8"/>
-        </left>
-        <right style="thin">
-          <color indexed="8"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="8"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="8"/>
-        </left>
-        <right style="thin">
-          <color indexed="8"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="8"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
         <color theme="1"/>
-        <family val="2"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
@@ -591,23 +479,139 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="8"/>
         </left>
         <right style="thin">
           <color indexed="8"/>
         </right>
-        <top style="thin">
-          <color indexed="8"/>
-        </top>
+        <top/>
         <bottom style="thin">
           <color indexed="8"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="8"/>
+        </left>
+        <right style="thin">
+          <color indexed="8"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="8"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="8"/>
+        </left>
+        <right style="thin">
+          <color indexed="8"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="8"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="8"/>
+        </left>
+        <right style="thin">
+          <color indexed="8"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="8"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="8"/>
+        </left>
+        <right style="thin">
+          <color indexed="8"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="8"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="8"/>
+        </left>
+        <right style="thin">
+          <color indexed="8"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="8"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="8"/>
+        </left>
+        <right style="thin">
+          <color indexed="8"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="8"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="8"/>
+        </left>
+        <right style="thin">
+          <color indexed="8"/>
+        </right>
+        <top style="thin">
+          <color indexed="8"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="8"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -654,19 +658,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla14515" displayName="Tabla14515" ref="A5:J6" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10">
-  <autoFilter ref="A5:J6" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabla14515" displayName="Tabla14515" ref="A5:J6" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="A5:J6"/>
   <tableColumns count="10">
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Student" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Lab 0, 1.1, 1.2" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Lab 2 (Sorting)" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Lab 3 (D&amp;C)" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Lab 4 (Greedy)" dataDxfId="1"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Lab 5 (Dynamic Prog.)" dataDxfId="0"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Lab 6 (Backtracking)" dataDxfId="5"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Lab 7 (Branch&amp;Bound)" dataDxfId="6"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Test mark" dataDxfId="7"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Final mark" dataDxfId="9" dataCellStyle="Normal">
+    <tableColumn id="3" name="Student" dataDxfId="9"/>
+    <tableColumn id="13" name="Lab 0, 1.1, 1.2" dataDxfId="8"/>
+    <tableColumn id="14" name="Lab 2 (Sorting)" dataDxfId="7"/>
+    <tableColumn id="15" name="Lab 3 (D&amp;C)" dataDxfId="6"/>
+    <tableColumn id="16" name="Lab 4 (Greedy)" dataDxfId="5"/>
+    <tableColumn id="17" name="Lab 5 (Dynamic Prog.)" dataDxfId="4"/>
+    <tableColumn id="18" name="Lab 6 (Backtracking)" dataDxfId="3"/>
+    <tableColumn id="19" name="Lab 7 (Branch&amp;Bound)" dataDxfId="2"/>
+    <tableColumn id="24" name="Test mark" dataDxfId="1"/>
+    <tableColumn id="21" name="Final mark" dataDxfId="0" dataCellStyle="Normal">
       <calculatedColumnFormula>IF(J4&lt;5,J4,IF(J4&lt;6,5,IF(J4&lt;7,5.5,IF(J4&lt;8,6,IF(J4&lt;9,6.5,IF(J4&lt;=10,7,100))))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -750,23 +754,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -802,23 +789,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1002,11 +972,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1026,49 +996,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="J3" s="11"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>0.1</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>0.1</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>0.15</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>0.15</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>0.15</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>0.2</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="6">
         <v>0.15</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="12">
         <f>B6*B4+C6*C4+D6*D4+E6*E4+F6*F4+G6*G4+H6*H4</f>
         <v>0</v>
       </c>
@@ -1077,150 +1047,150 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="13">
+      <c r="A6" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="9">
         <f>IF(J4&lt;5,J4,IF(J4&lt;6,5,IF(J4&lt;7,5.5,IF(J4&lt;8,6,IF(J4&lt;9,6.5,IF(J4&lt;=10,7,100))))))</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
     </row>
     <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
     </row>
     <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
     </row>
     <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
     </row>
     <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
     </row>
     <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>14</v>
+      <c r="A19" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>